<commit_message>
adding even more photos
</commit_message>
<xml_diff>
--- a/data/dilutions-aug-21-2018.xlsx
+++ b/data/dilutions-aug-21-2018.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16100" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>Dilution</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>total volume required</t>
+  </si>
+  <si>
+    <t>population_density</t>
   </si>
 </sst>
 </file>
@@ -432,326 +435,353 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.5" customWidth="1"/>
-    <col min="2" max="2" width="7.5" customWidth="1"/>
-    <col min="3" max="3" width="14.5" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" customWidth="1"/>
-    <col min="5" max="5" width="9.1640625" customWidth="1"/>
-    <col min="6" max="6" width="7.33203125" customWidth="1"/>
-    <col min="7" max="7" width="7.6640625" customWidth="1"/>
-    <col min="8" max="8" width="15.83203125" customWidth="1"/>
+    <col min="2" max="2" width="10.5" customWidth="1"/>
+    <col min="3" max="3" width="7.5" customWidth="1"/>
+    <col min="4" max="4" width="14.5" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" customWidth="1"/>
+    <col min="6" max="6" width="9.1640625" customWidth="1"/>
+    <col min="7" max="7" width="7.33203125" customWidth="1"/>
+    <col min="8" max="8" width="7.6640625" customWidth="1"/>
+    <col min="9" max="9" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="62" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:10" ht="62" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="2"/>
-    </row>
-    <row r="2" spans="1:9" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="J1" s="2"/>
+    </row>
+    <row r="2" spans="1:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4">
         <f>1/1</f>
         <v>1</v>
       </c>
-      <c r="C2" s="4">
-        <f>15*B2</f>
+      <c r="D2" s="4">
+        <f>15*C2</f>
         <v>15</v>
       </c>
-      <c r="D2" s="4">
-        <f>15-C2</f>
+      <c r="E2" s="4">
+        <f>15-D2</f>
         <v>0</v>
       </c>
-      <c r="E2" s="4"/>
       <c r="F2" s="4"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5">
+      <c r="G2" s="4"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5">
         <v>13.2</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="19" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="4">
         <f>1/1.5</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="C3" s="4">
-        <f>15*B3</f>
+      <c r="D3" s="4">
+        <f>15*C3</f>
         <v>10</v>
       </c>
-      <c r="D3" s="4">
-        <f t="shared" ref="D3:D9" si="0">15-C3</f>
+      <c r="E3" s="4">
+        <f t="shared" ref="E3:E9" si="0">15-D3</f>
         <v>5</v>
       </c>
-      <c r="E3" s="4"/>
       <c r="F3" s="4"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5">
+      <c r="G3" s="4"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5">
         <v>13.2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="19" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="4">
         <f>1/2</f>
         <v>0.5</v>
       </c>
-      <c r="C4" s="4">
-        <f t="shared" ref="C4:C9" si="1">15*B4</f>
+      <c r="D4" s="4">
+        <f t="shared" ref="D4:D9" si="1">15*C4</f>
         <v>7.5</v>
       </c>
-      <c r="D4" s="4">
+      <c r="E4" s="4">
         <f t="shared" si="0"/>
         <v>7.5</v>
       </c>
-      <c r="E4" s="4"/>
       <c r="F4" s="4"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5">
+      <c r="G4" s="4"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5">
         <v>13.2</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="19" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="4">
         <f>1/5</f>
         <v>0.2</v>
       </c>
-      <c r="C5" s="4">
+      <c r="D5" s="4">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="D5" s="4">
+      <c r="E5" s="4">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="E5" s="4"/>
       <c r="F5" s="4"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5">
+      <c r="G5" s="4"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5">
         <v>13.2</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="19" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="4">
         <f>1/10</f>
         <v>0.1</v>
       </c>
-      <c r="C6" s="4">
+      <c r="D6" s="4">
         <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
-      <c r="D6" s="4">
+      <c r="E6" s="4">
         <f t="shared" si="0"/>
         <v>13.5</v>
       </c>
-      <c r="E6" s="4"/>
       <c r="F6" s="4"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5">
+      <c r="G6" s="4"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5">
         <v>13.2</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="19" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+    <row r="7" spans="1:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="6">
+      <c r="C7" s="6">
         <f>1/20</f>
         <v>0.05</v>
       </c>
-      <c r="C7" s="6">
+      <c r="D7" s="6">
         <f t="shared" si="1"/>
         <v>0.75</v>
       </c>
-      <c r="D7" s="6">
+      <c r="E7" s="6">
         <f t="shared" si="0"/>
         <v>14.25</v>
       </c>
-      <c r="E7" s="6">
+      <c r="F7" s="6">
         <f>1.5</f>
         <v>1.5</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="G7" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G7" s="6">
-        <f>15-E7</f>
+      <c r="H7" s="6">
+        <f>15-F7</f>
         <v>13.5</v>
       </c>
-      <c r="H7" s="7">
+      <c r="I7" s="7">
         <v>13.2</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="19" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+    <row r="8" spans="1:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="6">
+      <c r="C8" s="6">
         <f>1/100</f>
         <v>0.01</v>
       </c>
-      <c r="C8" s="6">
+      <c r="D8" s="6">
         <f t="shared" si="1"/>
         <v>0.15</v>
       </c>
-      <c r="D8" s="6">
+      <c r="E8" s="6">
         <f t="shared" si="0"/>
         <v>14.85</v>
       </c>
-      <c r="E8" s="6">
+      <c r="F8" s="6">
         <v>1.5</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="G8" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G8" s="7">
+      <c r="H8" s="7">
         <v>13.5</v>
       </c>
-      <c r="H8" s="7">
+      <c r="I8" s="7">
         <v>13.2</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="19" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+    <row r="9" spans="1:10" ht="19" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="6">
+      <c r="C9" s="6">
         <f>1/1000</f>
         <v>1E-3</v>
       </c>
-      <c r="C9" s="6">
+      <c r="D9" s="6">
         <f t="shared" si="1"/>
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="D9" s="6">
+      <c r="E9" s="6">
         <f t="shared" si="0"/>
         <v>14.984999999999999</v>
       </c>
-      <c r="E9" s="6">
+      <c r="F9" s="6">
         <v>1.5</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="G9" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="7">
+      <c r="H9" s="7">
         <v>13.5</v>
       </c>
-      <c r="H9" s="7">
+      <c r="I9" s="7">
         <v>13.2</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="1"/>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="1"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="1"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="1"/>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="1"/>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="1"/>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="1"/>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="1"/>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="1"/>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>